<commit_message>
correction injection Excell pom + mise en place flyway
</commit_message>
<xml_diff>
--- a/distriWebApp/web/src/main/resources/annexes/importCocktail.xlsx
+++ b/distriWebApp/web/src/main/resources/annexes/importCocktail.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DOCUMENT\PERSO\workspaceDis\myprojectDistributeur2\distriWebApp\web\src\main\resources\annexes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="135" windowWidth="23715" windowHeight="9795" activeTab="1"/>
   </bookViews>
@@ -77,8 +82,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,15 +283,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -294,6 +290,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -305,21 +310,57 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -366,7 +407,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,9 +439,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -432,6 +474,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -607,14 +650,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
@@ -624,7 +667,7 @@
     <col min="6" max="6" width="14.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -644,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -664,7 +707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -684,7 +727,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -692,7 +735,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -700,7 +743,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -708,7 +751,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -716,7 +759,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -724,7 +767,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -732,7 +775,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -740,7 +783,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -748,7 +791,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -756,7 +799,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -764,7 +807,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -772,7 +815,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -780,7 +823,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -788,7 +831,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -796,7 +839,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -804,7 +847,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -812,7 +855,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -820,7 +863,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -828,7 +871,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -836,7 +879,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -844,7 +887,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -852,7 +895,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -860,7 +903,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -868,7 +911,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -876,7 +919,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -884,7 +927,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -892,7 +935,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -900,7 +943,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -908,7 +951,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -916,7 +959,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -924,7 +967,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -932,7 +975,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -940,7 +983,7 @@
       <c r="E35" s="2"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" thickBot="1">
+    <row r="36" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -954,14 +997,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
@@ -971,39 +1014,39 @@
     <col min="6" max="6" width="25.85546875" style="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="28"/>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1">
-      <c r="A2" s="29" t="s">
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1023,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
@@ -1037,7 +1080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1057,7 +1100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
@@ -1071,7 +1114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
@@ -1079,7 +1122,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
@@ -1087,7 +1130,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
@@ -1095,7 +1138,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="17"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
@@ -1103,7 +1146,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="17"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
@@ -1111,7 +1154,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="17"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
@@ -1119,7 +1162,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="17"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
@@ -1127,7 +1170,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="17"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
@@ -1135,7 +1178,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="17"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
@@ -1143,7 +1186,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
@@ -1151,7 +1194,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="17"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
@@ -1159,7 +1202,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="17"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
@@ -1167,7 +1210,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="17"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
@@ -1175,7 +1218,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="17"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
@@ -1183,7 +1226,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="17"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
@@ -1191,7 +1234,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="17"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
@@ -1199,7 +1242,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
@@ -1207,7 +1250,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="17"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
@@ -1215,7 +1258,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="17"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
@@ -1223,7 +1266,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="17"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
@@ -1231,7 +1274,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="17"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
@@ -1239,7 +1282,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="17"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
@@ -1247,7 +1290,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
@@ -1255,7 +1298,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="17"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
@@ -1263,7 +1306,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
@@ -1271,7 +1314,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="17"/>
     </row>
-    <row r="32" spans="1:6" ht="15.75" thickBot="1">
+    <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="9"/>

</xml_diff>